<commit_message>
Agregro Cronograma actualizado a esta fecha mas Resumenes Teoricos
</commit_message>
<xml_diff>
--- a/Produccion Propia/Cronogramas/Cronograma_Actividades_Grupales.xlsx
+++ b/Produccion Propia/Cronogramas/Cronograma_Actividades_Grupales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
   <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Facu\4º año\Ingenieria de Software (ISW)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00750A4-7262-4808-BF70-A7DB10E95688}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14E70981-384B-42F0-848C-6EF3F93F77E8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9510" tabRatio="741" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="720" uniqueCount="70">
   <si>
     <t>Día de la semana</t>
   </si>
@@ -310,6 +310,18 @@
   </si>
   <si>
     <t>1er Teorico Grupal - Pecha Kucha; Nota: 7 temas al parcial Teoricos Papers: No hay Balas de Plata y  Snowden HBR Cynefin A Leader’s Framework for Decision Making Color</t>
+  </si>
+  <si>
+    <t>Clase Teorica de Proceso de SW</t>
+  </si>
+  <si>
+    <t>Clase Teorica de  Consultas antes del parcial</t>
+  </si>
+  <si>
+    <t>Clase Practica de Reviciones tecnicas, comienzo del TP7 Entregable</t>
+  </si>
+  <si>
+    <t>Entregar TP7 de Reviciones Tecnicas</t>
   </si>
 </sst>
 </file>
@@ -7517,7 +7529,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="84" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28:H28"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8355,7 +8367,7 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="84" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8490,8 +8502,12 @@
         <v>43233</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="49"/>
+      <c r="K4" s="36">
+        <v>14</v>
+      </c>
+      <c r="L4" s="49" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
@@ -8646,8 +8662,12 @@
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="10"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="49"/>
+      <c r="K9" s="36">
+        <v>8</v>
+      </c>
+      <c r="L9" s="49" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
@@ -8962,8 +8982,12 @@
       <c r="J26" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="K26" s="37"/>
-      <c r="L26" s="49"/>
+      <c r="K26" s="37">
+        <v>4</v>
+      </c>
+      <c r="L26" s="49" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="26" t="s">
@@ -8978,8 +9002,12 @@
       <c r="H27" s="69"/>
       <c r="I27" s="54"/>
       <c r="J27" s="10"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="49"/>
+      <c r="K27" s="36">
+        <v>11</v>
+      </c>
+      <c r="L27" s="49" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="28" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="26" t="s">

</xml_diff>